<commit_message>
add driver file and functionality for different start row and col
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
-    <sheet name="blank" sheetId="1" r:id="rId1"/>
-    <sheet name="standard" sheetId="2" r:id="rId2"/>
-    <sheet name="headeronly" sheetId="3" r:id="rId3"/>
+    <sheet name="colrow2" sheetId="5" r:id="rId1"/>
+    <sheet name="headerrow2" sheetId="4" r:id="rId2"/>
+    <sheet name="blank" sheetId="1" r:id="rId3"/>
+    <sheet name="standard" sheetId="2" r:id="rId4"/>
+    <sheet name="headeronly" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
   <si>
     <t>uid</t>
   </si>
@@ -358,6 +360,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -368,7 +456,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -412,11 +500,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove new line characters from headers
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="colrow2" sheetId="5" r:id="rId1"/>
     <sheet name="headerrow2" sheetId="4" r:id="rId2"/>
     <sheet name="blank" sheetId="1" r:id="rId3"/>
     <sheet name="standard" sheetId="2" r:id="rId4"/>
-    <sheet name="headeronly" sheetId="3" r:id="rId5"/>
+    <sheet name="twolineheader" sheetId="6" r:id="rId5"/>
+    <sheet name="headeronly" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>uid</t>
   </si>
@@ -43,6 +44,10 @@
   </si>
   <si>
     <t>henry</t>
+  </si>
+  <si>
+    <t>two
+lines</t>
   </si>
 </sst>
 </file>
@@ -78,8 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,7 +370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -502,6 +510,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
remove all special characters from headers
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>uid</t>
   </si>
@@ -48,6 +48,9 @@
   <si>
     <t>two
 lines</t>
+  </si>
+  <si>
+    <t>m'"\ a</t>
   </si>
 </sst>
 </file>
@@ -510,22 +513,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>